<commit_message>
Added How To Release Lib Android
</commit_message>
<xml_diff>
--- a/Android/HowToReleaseLib_Android.xlsx
+++ b/Android/HowToReleaseLib_Android.xlsx
@@ -1,43 +1,105 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21727"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="A:\document\my_project\git\material\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Data\AppliDesign\IEI\git\Material\Android\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DE3DDA5-DB28-4F2C-8666-BB39C6589770}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4045A37-91B8-4250-9769-87A4B99FBC97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{222586B3-5BB9-47EA-981D-895DEA5CC057}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="29020" windowHeight="17500" xr2:uid="{222586B3-5BB9-47EA-981D-895DEA5CC057}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="MavenCentral" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="15">
   <si>
-    <t>ProgressBar</t>
+    <t>File -&gt; New -&gt; New Project</t>
   </si>
   <si>
-    <t>https://developer.android.com/reference/android/widget/ProgressBar.html</t>
+    <t>Add a Module Library</t>
+  </si>
+  <si>
+    <t>Create an App Project</t>
+  </si>
+  <si>
+    <t>File -&gt; New -&gt; New Module</t>
+  </si>
+  <si>
+    <t>C:\Users\UserName\.gradle\gradle.properties</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Get </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>signing.keyId</t>
+    </r>
+  </si>
+  <si>
+    <t>Execute this check whether the key is already generated or not</t>
+  </si>
+  <si>
+    <t>Add this to the file:</t>
+  </si>
+  <si>
+    <t>Output example:</t>
+  </si>
+  <si>
+    <t>If it is not generated yet, then generate the ID using this command:</t>
+  </si>
+  <si>
+    <t>3.1.1</t>
+  </si>
+  <si>
+    <t>Release Setting</t>
+  </si>
+  <si>
+    <t>Enter your name</t>
+  </si>
+  <si>
+    <t>Enter your email address</t>
+  </si>
+  <si>
+    <t>Enter and re-enter PassPhrase:</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -53,6 +115,35 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -77,9 +168,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -96,6 +190,1142 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>398700</xdr:colOff>
+      <xdr:row>79</xdr:row>
+      <xdr:rowOff>120600</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7A960C0F-3CFF-416E-9F2A-824BD530C101}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="495300" y="7918450"/>
+          <a:ext cx="10800000" cy="6750000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>398700</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>120600</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Picture 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{88B7E563-886D-4D08-A5EA-DB78C83C4B5D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="495300" y="552450"/>
+          <a:ext cx="10800000" cy="6750000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>131</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>68500</xdr:colOff>
+      <xdr:row>167</xdr:row>
+      <xdr:rowOff>120600</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="11" name="Picture 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{57B2EE34-A3D8-4746-E615-BC81A776B25E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="660400" y="15284450"/>
+          <a:ext cx="10800000" cy="6750000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>50800</xdr:colOff>
+      <xdr:row>84</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>469900</xdr:colOff>
+      <xdr:row>87</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="13" name="Rectangle 12">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{296BF0C9-95D1-F025-DDE8-FC3D6DF38C6C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="996950" y="23831550"/>
+          <a:ext cx="4076700" cy="641350"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0"/>
+            <a:t>--------------------------------Command Prompt---------------------------------</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100" b="0"/>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0"/>
+            <a:t>gpg --list-keys --keyid-format short</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100" b="0">
+            <a:solidFill>
+              <a:schemeClr val="lt1"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>90</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>95</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="17" name="Rectangle 16">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9A8DA447-14BE-4F3D-A958-5F7387F7D568}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="946150" y="24860250"/>
+          <a:ext cx="4305300" cy="977900"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="l" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>pub   ed25449/G9SDGAS8 2024-01-03 [SC] [</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="ja-JP" altLang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>有効期限</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>: 2027-01-02]</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="l" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>          4</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>C50F16C06E72AFC9BBEF1D7ADSFASDG9SDGAS8</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="l" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>uid         [  </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="ja-JP" altLang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>究極  </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>] </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>fwhyn &lt;fwhynseventh@gmail.com&gt;</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="l" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>sub   cv25519/8ED34GF 2024-01-03 [E] [</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="ja-JP" altLang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>有効期限</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>: 2027-01-02]</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>169</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>463550</xdr:colOff>
+      <xdr:row>172</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="19" name="Rectangle 18">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8A06601C-EAD1-4B80-929F-6F991FEB2380}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1143000" y="22282150"/>
+          <a:ext cx="4730750" cy="666750"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="l" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>signing.keyId=GpgShortKeyId</a:t>
+          </a:r>
+          <a:br>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+          </a:br>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>signing.password=PassPhrase</a:t>
+          </a:r>
+          <a:br>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+          </a:br>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>signing.secretKeyRingFile=C\:/Users/UserName/.gnupg/secring.gpg</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>97</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>419100</xdr:colOff>
+      <xdr:row>100</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="21" name="Rectangle 20">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{53A95C9D-E234-428B-B535-C810C3950131}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1143000" y="17862550"/>
+          <a:ext cx="4076700" cy="641350"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0"/>
+            <a:t>--------------------------------Command Prompt---------------------------------</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100" b="0"/>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0"/>
+            <a:t>gpg --gen-key</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100" b="0">
+            <a:solidFill>
+              <a:schemeClr val="lt1"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>104</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>520883</xdr:colOff>
+      <xdr:row>117</xdr:row>
+      <xdr:rowOff>127130</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="23" name="Picture 22">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EF380B3E-2779-43AA-A4DC-E1CE489814EA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1143000" y="19151600"/>
+          <a:ext cx="3568883" cy="2521080"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>66117</xdr:colOff>
+      <xdr:row>104</xdr:row>
+      <xdr:rowOff>6350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>578033</xdr:colOff>
+      <xdr:row>117</xdr:row>
+      <xdr:rowOff>133480</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="24" name="Picture 23">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{370D9C82-A15C-C236-264E-E8F36E573B15}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4866717" y="19157950"/>
+          <a:ext cx="3559916" cy="2521080"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>90</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>95</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="26" name="Rectangle 25">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ECE68979-34B5-4524-B682-BC6B5AEB54ED}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6629400" y="16573500"/>
+          <a:ext cx="4305300" cy="977900"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="l" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>pub   ed25449/GpgShortKeyId 2024-01-03 [SC] [</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="ja-JP" altLang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>有効期限</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>: 2027-01-02]</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="l" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>          </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>GpgFullKeyId</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="l" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>uid         [  </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="ja-JP" altLang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>究極  </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>] </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>fwhyn &lt;fwhynseventh@gmail.com&gt;</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="l" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>sub   cv25519/8EDF213C 2024-01-03 [E] [</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="ja-JP" altLang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>有効期限</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>: 2027-01-02]</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>361950</xdr:colOff>
+      <xdr:row>90</xdr:row>
+      <xdr:rowOff>107950</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>355600</xdr:colOff>
+      <xdr:row>94</xdr:row>
+      <xdr:rowOff>139700</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="27" name="Arrow: Right 26">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D74634E3-31CC-C499-13BB-92EEFDA84EDC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5772150" y="16681450"/>
+          <a:ext cx="603250" cy="768350"/>
+        </a:xfrm>
+        <a:prstGeom prst="rightArrow">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -395,31 +1625,125 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6DBECE46-0004-4AB9-A50E-F1B658391690}">
-  <dimension ref="B2:B3"/>
+  <dimension ref="B2:E169"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" topLeftCell="A87" workbookViewId="0">
+      <selection activeCell="I178" sqref="I178"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="3.5703125" customWidth="1"/>
+    <col min="1" max="2" width="3.54296875" customWidth="1"/>
+    <col min="3" max="3" width="4" customWidth="1"/>
+    <col min="4" max="4" width="5.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B2" t="s">
+    <row r="2" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B2" s="2">
+        <v>1</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B3" s="1"/>
+      <c r="C3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B3" s="1" t="s">
+    <row r="42" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B42" s="2">
+        <v>2</v>
+      </c>
+      <c r="C42" s="2" t="s">
         <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="C43" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="82" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B82" s="2">
+        <v>3</v>
+      </c>
+      <c r="C82" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="83" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="C83">
+        <v>3.1</v>
+      </c>
+      <c r="D83" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="84" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="D84" t="s">
+        <v>10</v>
+      </c>
+      <c r="E84" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="85" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="E85" s="4"/>
+    </row>
+    <row r="90" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="E90" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="97" spans="4:5" x14ac:dyDescent="0.35">
+      <c r="D97" t="s">
+        <v>10</v>
+      </c>
+      <c r="E97" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="102" spans="4:5" x14ac:dyDescent="0.35">
+      <c r="E102" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="103" spans="4:5" x14ac:dyDescent="0.35">
+      <c r="E103" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="104" spans="4:5" x14ac:dyDescent="0.35">
+      <c r="E104" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="131" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D131" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="169" spans="4:5" x14ac:dyDescent="0.35">
+      <c r="D169" t="s">
+        <v>10</v>
+      </c>
+      <c r="E169" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B3" r:id="rId1" xr:uid="{D6336836-DEE7-46E3-B598-E57611E16A30}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter>
+    <oddFooter>&amp;L_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Internal</oddFooter>
+  </headerFooter>
+  <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
+<clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
+  <clbl:label id="{549229e1-d9eb-40cf-aa20-8039fe5d6144}" enabled="1" method="Standard" siteId="{3ce358ea-700e-4f0f-bb37-fd0b7c21366c}" contentBits="2" removed="0"/>
+</clbl:labelList>
 </file>
</xml_diff>

<commit_message>
How To Release Lib Android
</commit_message>
<xml_diff>
--- a/Android/HowToReleaseLib_Android.xlsx
+++ b/Android/HowToReleaseLib_Android.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Data\AppliDesign\IEI\git\Material\Android\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4045A37-91B8-4250-9769-87A4B99FBC97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{987ADC27-A4A9-47B4-8A3D-A30B3DE35AC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="29020" windowHeight="17500" xr2:uid="{222586B3-5BB9-47EA-981D-895DEA5CC057}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>File -&gt; New -&gt; New Project</t>
   </si>
@@ -51,6 +51,36 @@
   </si>
   <si>
     <t>C:\Users\UserName\.gradle\gradle.properties</t>
+  </si>
+  <si>
+    <t>Execute this check whether the key is already generated or not</t>
+  </si>
+  <si>
+    <t>Add this to the file:</t>
+  </si>
+  <si>
+    <t>Output example:</t>
+  </si>
+  <si>
+    <t>If it is not generated yet, then generate the ID using this command:</t>
+  </si>
+  <si>
+    <t>3.1.1</t>
+  </si>
+  <si>
+    <t>Release Setting</t>
+  </si>
+  <si>
+    <t>Enter your name</t>
+  </si>
+  <si>
+    <t>Enter your email address</t>
+  </si>
+  <si>
+    <t>Enter and re-enter PassPhrase:</t>
+  </si>
+  <si>
+    <t>Set the GPG</t>
   </si>
   <si>
     <r>
@@ -64,35 +94,35 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>signing.keyId</t>
+      <t>GPG ID</t>
     </r>
   </si>
   <si>
-    <t>Execute this check whether the key is already generated or not</t>
-  </si>
-  <si>
-    <t>Add this to the file:</t>
-  </si>
-  <si>
-    <t>Output example:</t>
-  </si>
-  <si>
-    <t>If it is not generated yet, then generate the ID using this command:</t>
-  </si>
-  <si>
-    <t>3.1.1</t>
-  </si>
-  <si>
-    <t>Release Setting</t>
-  </si>
-  <si>
-    <t>Enter your name</t>
-  </si>
-  <si>
-    <t>Enter your email address</t>
-  </si>
-  <si>
-    <t>Enter and re-enter PassPhrase:</t>
+    <t>3.1.2</t>
+  </si>
+  <si>
+    <t>then run step 3.1.1 again</t>
+  </si>
+  <si>
+    <t>3.1.3</t>
+  </si>
+  <si>
+    <t>Generate Secring.gpg</t>
+  </si>
+  <si>
+    <t>Execute this command</t>
+  </si>
+  <si>
+    <t>copy generated result to</t>
+  </si>
+  <si>
+    <t>C:\Users\UserName\.gnupg</t>
+  </si>
+  <si>
+    <t>Set for POM properties</t>
+  </si>
+  <si>
+    <t>\YourLibProjectName\gradle.properties</t>
   </si>
 </sst>
 </file>
@@ -286,13 +316,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>131</xdr:row>
+      <xdr:row>133</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>21</xdr:col>
       <xdr:colOff>68500</xdr:colOff>
-      <xdr:row>167</xdr:row>
+      <xdr:row>169</xdr:row>
       <xdr:rowOff>120600</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -679,139 +709,6 @@
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
             <a:t>: 2027-01-02]</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>169</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>463550</xdr:colOff>
-      <xdr:row>172</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="19" name="Rectangle 18">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8A06601C-EAD1-4B80-929F-6F991FEB2380}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="1143000" y="22282150"/>
-          <a:ext cx="4730750" cy="666750"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="15000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="l" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
-            <a:lnSpc>
-              <a:spcPct val="100000"/>
-            </a:lnSpc>
-            <a:spcBef>
-              <a:spcPts val="0"/>
-            </a:spcBef>
-            <a:spcAft>
-              <a:spcPts val="0"/>
-            </a:spcAft>
-            <a:buClrTx/>
-            <a:buSzTx/>
-            <a:buFontTx/>
-            <a:buNone/>
-            <a:tabLst/>
-            <a:defRPr/>
-          </a:pPr>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100">
-              <a:solidFill>
-                <a:schemeClr val="lt1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>signing.keyId=GpgShortKeyId</a:t>
-          </a:r>
-          <a:br>
-            <a:rPr lang="en-US" sz="1100">
-              <a:solidFill>
-                <a:schemeClr val="lt1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-          </a:br>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100">
-              <a:solidFill>
-                <a:schemeClr val="lt1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>signing.password=PassPhrase</a:t>
-          </a:r>
-          <a:br>
-            <a:rPr lang="en-US" sz="1100">
-              <a:solidFill>
-                <a:schemeClr val="lt1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-          </a:br>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100">
-              <a:solidFill>
-                <a:schemeClr val="lt1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>signing.secretKeyRingFile=C\:/Users/UserName/.gnupg/secring.gpg</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -1069,7 +966,31 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>pub   ed25449/GpgShortKeyId 2024-01-03 [SC] [</a:t>
+            <a:t>pub   ed25449/</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>GpgShortKeyId</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t> 2024-01-03 [SC] [</a:t>
           </a:r>
           <a:r>
             <a:rPr lang="ja-JP" altLang="en-US" sz="1100">
@@ -1127,7 +1048,7 @@
             <a:t>          </a:t>
           </a:r>
           <a:r>
-            <a:rPr lang="en-US" sz="1100">
+            <a:rPr lang="en-US" sz="1100" b="1">
               <a:solidFill>
                 <a:schemeClr val="lt1"/>
               </a:solidFill>
@@ -1268,19 +1189,19 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>361950</xdr:colOff>
+      <xdr:colOff>228600</xdr:colOff>
       <xdr:row>90</xdr:row>
-      <xdr:rowOff>107950</xdr:rowOff>
+      <xdr:rowOff>139700</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>355600</xdr:colOff>
+      <xdr:colOff>482600</xdr:colOff>
       <xdr:row>94</xdr:row>
-      <xdr:rowOff>139700</xdr:rowOff>
+      <xdr:rowOff>171450</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="27" name="Arrow: Right 26">
+        <xdr:cNvPr id="27" name="Arrow: Left-Right 26">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
               <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D74634E3-31CC-C499-13BB-92EEFDA84EDC}"/>
@@ -1291,11 +1212,14 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5772150" y="16681450"/>
-          <a:ext cx="603250" cy="768350"/>
+          <a:off x="5638800" y="16713200"/>
+          <a:ext cx="863600" cy="768350"/>
         </a:xfrm>
-        <a:prstGeom prst="rightArrow">
-          <a:avLst/>
+        <a:prstGeom prst="leftRightArrow">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 41735"/>
+            <a:gd name="adj2" fmla="val 34298"/>
+          </a:avLst>
         </a:prstGeom>
       </xdr:spPr>
       <xdr:style>
@@ -1323,6 +1247,266 @@
         </a:p>
       </xdr:txBody>
     </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>123</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>419100</xdr:colOff>
+      <xdr:row>126</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="Rectangle 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{78C561FD-4F65-4589-8358-B59725FFEBCC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1143000" y="22650450"/>
+          <a:ext cx="4076700" cy="641350"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0"/>
+            <a:t>--------------------------------Command Prompt---------------------------------</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100" b="0"/>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0"/>
+            <a:t>gpg --export-secret-keys -o secring.gpg</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100" b="0">
+            <a:solidFill>
+              <a:schemeClr val="lt1"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>171</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>95250</xdr:colOff>
+      <xdr:row>174</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="Rectangle 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{41F30BCE-2E55-4327-B116-E16DBA24907E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="774700" y="31489650"/>
+          <a:ext cx="4730750" cy="666750"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="l" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>signing.keyId=GpgShortKeyId</a:t>
+          </a:r>
+          <a:br>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+          </a:br>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>signing.password=PassPhrase</a:t>
+          </a:r>
+          <a:br>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+          </a:br>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>signing.secretKeyRingFile=C\:/Users/UserName/.gnupg/secring.gpg</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>178</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>68500</xdr:colOff>
+      <xdr:row>214</xdr:row>
+      <xdr:rowOff>120600</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Picture 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FBB707C7-53A5-083B-73DB-4844516D95D1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="774700" y="32778700"/>
+          <a:ext cx="10800000" cy="6750000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -1625,10 +1809,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6DBECE46-0004-4AB9-A50E-F1B658391690}">
-  <dimension ref="B2:E169"/>
+  <dimension ref="B2:E178"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A87" workbookViewId="0">
-      <selection activeCell="I178" sqref="I178"/>
+    <sheetView tabSelected="1" topLeftCell="A172" workbookViewId="0">
+      <selection activeCell="R173" sqref="R173"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1670,7 +1854,7 @@
         <v>3</v>
       </c>
       <c r="C82" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="83" spans="2:5" x14ac:dyDescent="0.35">
@@ -1678,15 +1862,15 @@
         <v>3.1</v>
       </c>
       <c r="D83" s="3" t="s">
-        <v>5</v>
+        <v>15</v>
       </c>
     </row>
     <row r="84" spans="2:5" x14ac:dyDescent="0.35">
       <c r="D84" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E84" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="85" spans="2:5" x14ac:dyDescent="0.35">
@@ -1694,43 +1878,89 @@
     </row>
     <row r="90" spans="2:5" x14ac:dyDescent="0.35">
       <c r="E90" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="97" spans="4:5" x14ac:dyDescent="0.35">
       <c r="D97" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="E97" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="102" spans="4:5" x14ac:dyDescent="0.35">
       <c r="E102" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="103" spans="4:5" x14ac:dyDescent="0.35">
       <c r="E103" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="104" spans="4:5" x14ac:dyDescent="0.35">
       <c r="E104" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="120" spans="4:5" x14ac:dyDescent="0.35">
+      <c r="E120" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="122" spans="4:5" x14ac:dyDescent="0.35">
+      <c r="D122" t="s">
+        <v>18</v>
+      </c>
+      <c r="E122" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="123" spans="4:5" x14ac:dyDescent="0.35">
+      <c r="E123" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="129" spans="3:5" x14ac:dyDescent="0.35">
+      <c r="E129" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="130" spans="3:5" x14ac:dyDescent="0.35">
+      <c r="E130" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="132" spans="3:5" x14ac:dyDescent="0.35">
+      <c r="C132">
+        <v>3.2</v>
+      </c>
+      <c r="D132" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="131" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D131" t="s">
+    <row r="133" spans="3:5" x14ac:dyDescent="0.35">
+      <c r="D133" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="169" spans="4:5" x14ac:dyDescent="0.35">
-      <c r="D169" t="s">
-        <v>10</v>
-      </c>
-      <c r="E169" t="s">
-        <v>7</v>
+    <row r="171" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D171" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="177" spans="3:4" x14ac:dyDescent="0.35">
+      <c r="C177">
+        <v>3.3</v>
+      </c>
+      <c r="D177" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="178" spans="3:4" x14ac:dyDescent="0.35">
+      <c r="D178" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>